<commit_message>
add meir comments to grade file
</commit_message>
<xml_diff>
--- a/public/templates/grades.xlsx
+++ b/public/templates/grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\meir-att\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC731A-16DE-4CFD-8613-DE808D6A967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BB3F43-6EBC-4DCB-B9E9-0CD1B62843FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21948" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
   <sheets>
     <sheet name="גליון" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ת.ז.</t>
   </si>
@@ -69,20 +69,19 @@
     <t>${lesson.name}</t>
   </si>
   <si>
-    <r>
-      <t>התנהגות ,צניעות וכד' (הערות והארות</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
+    <t>התנהגות וד"א</t>
+  </si>
+  <si>
+    <t>צניעות</t>
+  </si>
+  <si>
+    <t>א=טובה מאוד, ב=פטפוט, ג=פטפוט כבד</t>
+  </si>
+  <si>
+    <t>א=טובה מאוד, ב=הערה אחת, ג=לא תואמת תקנון</t>
+  </si>
+  <si>
+    <t>הערות</t>
   </si>
 </sst>
 </file>
@@ -461,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0D8B3-8917-4C0C-99DA-1853A0CA42E9}">
-  <dimension ref="A1:G315"/>
+  <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -475,10 +474,11 @@
     <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -498,10 +498,16 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -515,8 +521,14 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -533,43 +545,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>